<commit_message>
added five variables in landsat sheet for hot/cold pixel calibration
</commit_message>
<xml_diff>
--- a/docs/InputEXCEL_v3_3_7_LIN.xlsx
+++ b/docs/InputEXCEL_v3_3_7_LIN.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="5748"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="5748" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="General_Input" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="78">
   <si>
     <t>InputMap</t>
   </si>
@@ -89,12 +89,6 @@
     <t>Method_radiation_inst</t>
   </si>
   <si>
-    <t>Hot_Pixel_Constant_Landsat</t>
-  </si>
-  <si>
-    <t>Cold_Pixel_Constant_Landsat</t>
-  </si>
-  <si>
     <t>Obstacle Height</t>
   </si>
   <si>
@@ -255,6 +249,21 @@
   </si>
   <si>
     <t>/mnt/d/PySebal/test_data/input/dem_dal.tif</t>
+  </si>
+  <si>
+    <t>tscold_min</t>
+  </si>
+  <si>
+    <t>tscold_max</t>
+  </si>
+  <si>
+    <t>ndvihot_low</t>
+  </si>
+  <si>
+    <t>ndvihot_high</t>
+  </si>
+  <si>
+    <t>temp_lapse_rate</t>
   </si>
 </sst>
 </file>
@@ -695,8 +704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -734,19 +743,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D2" s="4">
         <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -754,7 +763,7 @@
         <v>2</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -767,7 +776,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -775,7 +784,7 @@
         <v>4</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -783,7 +792,7 @@
         <v>5</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -791,7 +800,7 @@
         <v>6</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -799,7 +808,7 @@
         <v>7</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -829,56 +838,56 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B15" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C15" s="5"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B16" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -942,13 +951,13 @@
         <v>18</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O1" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -998,7 +1007,7 @@
         <v>0.4</v>
       </c>
       <c r="R2" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
@@ -1020,7 +1029,7 @@
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
       <c r="R3" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
@@ -1042,7 +1051,7 @@
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
       <c r="R4" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
@@ -1064,7 +1073,7 @@
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
       <c r="R5" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
@@ -1086,7 +1095,7 @@
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
       <c r="R6" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
@@ -1094,7 +1103,7 @@
         <v>6</v>
       </c>
       <c r="R7" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
@@ -1102,7 +1111,7 @@
         <v>7</v>
       </c>
       <c r="R8" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
@@ -1161,28 +1170,28 @@
         <v>3</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>25</v>
-      </c>
       <c r="F1" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G1" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="9" t="s">
         <v>54</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -1246,7 +1255,7 @@
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="K4" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -1262,7 +1271,7 @@
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="K5" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -1278,7 +1287,7 @@
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="K6" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -1286,7 +1295,7 @@
         <v>6</v>
       </c>
       <c r="K7" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -1294,7 +1303,7 @@
         <v>7</v>
       </c>
       <c r="K8" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
@@ -1332,8 +1341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1342,8 +1351,11 @@
     <col min="2" max="2" width="41.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="36.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1361,10 +1373,19 @@
         <v>7</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>19</v>
+        <v>73</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>20</v>
+        <v>74</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -1372,7 +1393,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C2" s="4">
         <v>8</v>
@@ -1381,13 +1402,22 @@
         <v>2</v>
       </c>
       <c r="E2" s="4">
-        <v>2</v>
+        <v>285</v>
       </c>
       <c r="F2" s="4">
-        <v>0.5</v>
+        <v>320</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0.03</v>
+      </c>
+      <c r="H2" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="I2" s="4">
+        <v>8.5000000000000006E-3</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -1400,7 +1430,7 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="J3" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -1413,7 +1443,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="J4" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -1421,7 +1451,7 @@
         <v>4</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -1430,7 +1460,7 @@
       </c>
       <c r="B6" s="4"/>
       <c r="J6" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -1438,7 +1468,7 @@
         <v>6</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -1446,7 +1476,7 @@
         <v>7</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -1505,22 +1535,22 @@
         <v>3</v>
       </c>
       <c r="B1" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="F1" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>29</v>
-      </c>
       <c r="G1" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -1528,11 +1558,11 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E2" s="4">
         <v>2</v>
@@ -1544,7 +1574,7 @@
         <v>36</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -1552,11 +1582,11 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E3" s="4">
         <v>2</v>
@@ -1568,7 +1598,7 @@
         <v>36</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -1582,7 +1612,7 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="I4" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -1590,7 +1620,7 @@
         <v>4</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -1598,7 +1628,7 @@
         <v>5</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -1606,7 +1636,7 @@
         <v>6</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -1614,7 +1644,7 @@
         <v>7</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -1668,22 +1698,22 @@
         <v>3</v>
       </c>
       <c r="B1" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>65</v>
-      </c>
       <c r="E1" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -1691,13 +1721,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E2" s="4">
         <v>2</v>
@@ -1746,19 +1776,19 @@
         <v>3</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>32</v>
-      </c>
       <c r="E1" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H1" s="4"/>
     </row>
@@ -1767,7 +1797,7 @@
         <v>1</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -1776,7 +1806,7 @@
       </c>
       <c r="B3" s="4"/>
       <c r="H3" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -1784,7 +1814,7 @@
         <v>3</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -1792,7 +1822,7 @@
         <v>4</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -1800,7 +1830,7 @@
         <v>5</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -1808,7 +1838,7 @@
         <v>6</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -1816,7 +1846,7 @@
         <v>7</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
added sample data to test the installation
</commit_message>
<xml_diff>
--- a/docs/InputEXCEL_v3_3_7_LIN.xlsx
+++ b/docs/InputEXCEL_v3_3_7_LIN.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="5748" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="5748"/>
   </bookViews>
   <sheets>
     <sheet name="General_Input" sheetId="1" r:id="rId1"/>
@@ -242,15 +242,6 @@
     <t>LC08_L1TP_173049_20140310_20170425_01_T1</t>
   </si>
   <si>
-    <t>/mnt/d/PySebal/test_data/input/insat</t>
-  </si>
-  <si>
-    <t>/mnt/d/PySebal/test_data/output</t>
-  </si>
-  <si>
-    <t>/mnt/d/PySebal/test_data/input/dem_dal.tif</t>
-  </si>
-  <si>
     <t>tscold_min</t>
   </si>
   <si>
@@ -264,6 +255,15 @@
   </si>
   <si>
     <t>temp_lapse_rate</t>
+  </si>
+  <si>
+    <t>/mnt/d/PySebal_dev/test_data/input/insat</t>
+  </si>
+  <si>
+    <t>/mnt/d/PySebal_dev/test_data/output</t>
+  </si>
+  <si>
+    <t>/mnt/d/PySebal_dev/test_data/input/dem_dal.tif</t>
   </si>
 </sst>
 </file>
@@ -704,8 +704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -743,16 +743,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="D2" s="4">
         <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>33</v>
@@ -1341,8 +1341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1373,19 +1373,19 @@
         <v>7</v>
       </c>
       <c r="E1" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="I1" s="10" t="s">
         <v>74</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -1402,19 +1402,19 @@
         <v>2</v>
       </c>
       <c r="E2" s="4">
-        <v>285</v>
+        <v>306.47000000000003</v>
       </c>
       <c r="F2" s="4">
-        <v>320</v>
+        <v>307.06</v>
       </c>
       <c r="G2" s="4">
-        <v>0.03</v>
+        <v>7.9000000000000001E-2</v>
       </c>
       <c r="H2" s="4">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="I2" s="4">
-        <v>8.5000000000000006E-3</v>
+        <v>6.4999999999999997E-3</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
minor change in excel file for linux
</commit_message>
<xml_diff>
--- a/docs/InputEXCEL_v3_3_7_LIN.xlsx
+++ b/docs/InputEXCEL_v3_3_7_LIN.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PySebal\PySEBAL_Pareeth\PySEBAL_dev\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PySEBAL_dev\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -257,13 +257,13 @@
     <t>temp_lapse_rate</t>
   </si>
   <si>
-    <t>/mnt/d/PySebal_dev/test_data/input/insat</t>
-  </si>
-  <si>
-    <t>/mnt/d/PySebal_dev/test_data/output</t>
-  </si>
-  <si>
-    <t>/mnt/d/PySebal_dev/test_data/input/dem_dal.tif</t>
+    <t>/mnt/d/PySEBAL_dev/test_data/input/insat</t>
+  </si>
+  <si>
+    <t>/mnt/d/PySEBAL_dev/test_data/output</t>
+  </si>
+  <si>
+    <t>/mnt/d/PySEBAL_dev/test_data/input/dem_dal.tif</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
added percentile based thresholding, removed two layers of caliba and run, saved into new version 3.7.8
</commit_message>
<xml_diff>
--- a/docs/InputEXCEL_v3_3_7_LIN.xlsx
+++ b/docs/InputEXCEL_v3_3_7_LIN.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PySEBAL_dev\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PySebal\PySEBAL_Pareeth\PySEBAL_dev\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="5748"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="5748" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="General_Input" sheetId="1" r:id="rId1"/>
@@ -257,13 +257,13 @@
     <t>temp_lapse_rate</t>
   </si>
   <si>
-    <t>/mnt/d/PySEBAL_dev/test_data/input/insat</t>
-  </si>
-  <si>
-    <t>/mnt/d/PySEBAL_dev/test_data/output</t>
-  </si>
-  <si>
-    <t>/mnt/d/PySEBAL_dev/test_data/input/dem_dal.tif</t>
+    <t>/mnt/d/PySEBAL/PySEBAL_Pareeth/PySEBAL_dev/test_data/input/insat</t>
+  </si>
+  <si>
+    <t>/mnt/d/PySEBAL/PySEBAL_Pareeth/PySEBAL_dev/test_data/output</t>
+  </si>
+  <si>
+    <t>/mnt/d/PySEBAL/PySEBAL_Pareeth/PySEBAL_dev/test_data/input/dem_dal.tif</t>
   </si>
 </sst>
 </file>
@@ -704,8 +704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1341,8 +1341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1402,16 +1402,16 @@
         <v>2</v>
       </c>
       <c r="E2" s="4">
-        <v>306.47000000000003</v>
+        <v>2</v>
       </c>
       <c r="F2" s="4">
-        <v>307.06</v>
+        <v>5</v>
       </c>
       <c r="G2" s="4">
-        <v>7.9000000000000001E-2</v>
+        <v>1</v>
       </c>
       <c r="H2" s="4">
-        <v>0.1</v>
+        <v>5</v>
       </c>
       <c r="I2" s="4">
         <v>6.4999999999999997E-3</v>

</xml_diff>

<commit_message>
change in syntax for ==
</commit_message>
<xml_diff>
--- a/docs/InputEXCEL_v3_3_7_LIN.xlsx
+++ b/docs/InputEXCEL_v3_3_7_LIN.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20374"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PySebal\PySEBAL_Pareeth\PySEBAL_dev\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PySEBAL_dev\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4138846A-E2DA-44AB-B67D-A5329055149C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="5748"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General_Input" sheetId="1" r:id="rId1"/>
@@ -260,16 +261,16 @@
     <t>/mnt/d/PySEBAL_dev/test_data/input/insat</t>
   </si>
   <si>
-    <t>/mnt/d/PySEBAL_dev/test_data/output</t>
-  </si>
-  <si>
     <t>/mnt/d/PySEBAL_dev/test_data/input/dem_dal.tif</t>
+  </si>
+  <si>
+    <t>/mnt/d/PySEBAL_dev/test_data/output_lin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -701,11 +702,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -746,13 +747,13 @@
         <v>75</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D2" s="4">
         <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>33</v>
@@ -897,7 +898,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1146,7 +1147,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1338,7 +1339,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1511,7 +1512,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -1679,7 +1680,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1755,7 +1756,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>